<commit_message>
Extracting Storage into jmeter-utils
</commit_message>
<xml_diff>
--- a/documentation/Examples/ExcelDataProvider/Excel_Data.xlsx
+++ b/documentation/Examples/ExcelDataProvider/Excel_Data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t xml:space="preserve">Field_1</t>
   </si>
@@ -71,40 +71,31 @@
     <t xml:space="preserve">D 13</t>
   </si>
   <si>
+    <t xml:space="preserve">D 14</t>
+  </si>
+  <si>
     <t xml:space="preserve">A 21</t>
   </si>
   <si>
-    <t xml:space="preserve">B 21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C 21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D 21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A 22</t>
-  </si>
-  <si>
     <t xml:space="preserve">B 22</t>
   </si>
   <si>
-    <t xml:space="preserve">C 22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D 22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A 23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B 23</t>
-  </si>
-  <si>
     <t xml:space="preserve">C 23</t>
   </si>
   <si>
-    <t xml:space="preserve">D 23</t>
+    <t xml:space="preserve">D 24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A 31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B 32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C 33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D 34</t>
   </si>
 </sst>
 </file>
@@ -212,7 +203,7 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7813765182186"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
@@ -297,7 +288,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -316,44 +307,44 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
only one problem left - It does not work witch cycles.
</commit_message>
<xml_diff>
--- a/documentation/Examples/ExcelDataProvider/Excel_Data.xlsx
+++ b/documentation/Examples/ExcelDataProvider/Excel_Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t xml:space="preserve">Field_1</t>
   </si>
@@ -59,43 +59,43 @@
     <t xml:space="preserve">D 12</t>
   </si>
   <si>
+    <t xml:space="preserve">C 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A 21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B 22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C 23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D 24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A 31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B 32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C 33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D 34</t>
+  </si>
+  <si>
     <t xml:space="preserve">A 13</t>
   </si>
   <si>
     <t xml:space="preserve">B 13</t>
   </si>
   <si>
-    <t xml:space="preserve">C 13</t>
-  </si>
-  <si>
     <t xml:space="preserve">D 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D 14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A 21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B 22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C 23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D 24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A 31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B 32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C 33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D 34</t>
   </si>
 </sst>
 </file>
@@ -193,17 +193,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.9959514170041"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
@@ -236,7 +236,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>8</v>
       </c>
@@ -248,20 +248,6 @@
       </c>
       <c r="D3" s="0" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -280,10 +266,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -313,37 +299,65 @@
         <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="0" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="B7" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="C7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Completed "reload" feature for DataController.
</commit_message>
<xml_diff>
--- a/documentation/Examples/ExcelDataProvider/Excel_Data.xlsx
+++ b/documentation/Examples/ExcelDataProvider/Excel_Data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t xml:space="preserve">Field_1</t>
   </si>
@@ -59,9 +59,18 @@
     <t xml:space="preserve">D 12</t>
   </si>
   <si>
+    <t xml:space="preserve">A 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B 13</t>
+  </si>
+  <si>
     <t xml:space="preserve">C 13</t>
   </si>
   <si>
+    <t xml:space="preserve">D 13</t>
+  </si>
+  <si>
     <t xml:space="preserve">D 14</t>
   </si>
   <si>
@@ -87,15 +96,6 @@
   </si>
   <si>
     <t xml:space="preserve">D 34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D 13</t>
   </si>
 </sst>
 </file>
@@ -193,17 +193,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1052631578947"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
@@ -248,6 +248,20 @@
       </c>
       <c r="D3" s="0" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -299,38 +313,38 @@
         <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -349,16 +363,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>